<commit_message>
Fixed some tire labels in TireInfo.xlsx
</commit_message>
<xml_diff>
--- a/TireInfo.xlsx
+++ b/TireInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\MATLAB\Projects\Tire Analyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F050447-93D8-473F-BE26-C9E25CDC5F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EA2A25-E1FC-4DE5-A9D0-B47B0D454937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{54157745-4C9D-4417-9AB7-640F59D95870}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{54157745-4C9D-4417-9AB7-640F59D95870}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="97">
   <si>
     <t>Goodyear 20x7-13</t>
   </si>
@@ -127,18 +127,6 @@
     <t>Michelin 16/53-13 on 8 in. wide rim</t>
   </si>
   <si>
-    <t>Hoosier 20.5x6.0-13 on 7 in. wide rim</t>
-  </si>
-  <si>
-    <t>Hoosier 20.5x6.0-13 on 8 in. wide rim</t>
-  </si>
-  <si>
-    <t>Hoosier 20x7.5-13 on 7 in. wide rim</t>
-  </si>
-  <si>
-    <t>Hoosier 20x7.5-13 on 8 in. wide rim</t>
-  </si>
-  <si>
     <t>Goodyear  D2704  20.0x7.0-13  on 7 in. wide rim</t>
   </si>
   <si>
@@ -172,24 +160,12 @@
     <t>Hoosier 20.5 x 6.0 13 R25B A2500 (Item 43127), 7 inch rim</t>
   </si>
   <si>
-    <t>Hoosier 20.5 x 7.0 13 R25B A2500 (Item 43127), 6 inch rim</t>
-  </si>
-  <si>
-    <t>Hoosier 20.5 x 7.0 13 R25B A2500 (Item 43127), 7 inch rim</t>
-  </si>
-  <si>
     <t>Continental 205/510R13 (4914), 7 inch rim</t>
   </si>
   <si>
     <t>Continental 205/510R13 (4914), 8 inch rim</t>
   </si>
   <si>
-    <t>Hoosier 18.0 x 7.5 10 R25B (Item 43105), 7 inch rim</t>
-  </si>
-  <si>
-    <t>Hoosier 18.0 x 7.5 10 R25B (Item 43105), 8 inch rim</t>
-  </si>
-  <si>
     <t>Hoosier 18.0 x 6.0 10 R25B (Item 43101), 6 inch rim</t>
   </si>
   <si>
@@ -229,15 +205,6 @@
     <t>Hoosier 43075 16x7.5-10 R25B, 7 inch rim</t>
   </si>
   <si>
-    <t>Hoosier 42070 16x6.0-10 R25B, 7 inch rim</t>
-  </si>
-  <si>
-    <t>Hoosier 42070 16x7.5-10 LCO, 7 inch rim</t>
-  </si>
-  <si>
-    <t>Hoosier 42070 16x6.0-10 LCO, 7 inch rim</t>
-  </si>
-  <si>
     <t>Continental 205/470R13 43329, 7 inch rim</t>
   </si>
   <si>
@@ -247,15 +214,6 @@
     <t>Hoosier 43075 16x7.5-10 R25B, 8 inch rim</t>
   </si>
   <si>
-    <t>Hoosier 42070 16x6.0-10 R25B, 6 inch rim</t>
-  </si>
-  <si>
-    <t>Hoosier 42070 16x7.5-10 LCO, 8 inch rim</t>
-  </si>
-  <si>
-    <t>Hoosier 42070 16x6.0-10 LCO, 6 inch rim</t>
-  </si>
-  <si>
     <t>Goodyear 20x7-13 D2704, 8 inch rim</t>
   </si>
   <si>
@@ -302,6 +260,69 @@
   </si>
   <si>
     <t>Tire_Name</t>
+  </si>
+  <si>
+    <t>Goodyear 20.0x7.0-13 "D2696" on 7 in. wide rim</t>
+  </si>
+  <si>
+    <t>Goodyear 20.0x7.0-13 "D2696" on 8 in. wide rim</t>
+  </si>
+  <si>
+    <t>Michelin 16/53-13 "Radial X S6B" on 7 in. wide rim</t>
+  </si>
+  <si>
+    <t>Michelin 16/53-13 "Radial X S6B" on 8 in. wide rim</t>
+  </si>
+  <si>
+    <t>Hoosier 20.5x6.0-13 R25B on 7 in. wide rim</t>
+  </si>
+  <si>
+    <t>Hoosier 20.5x7.0-13 R25B on 7 in. wide rim</t>
+  </si>
+  <si>
+    <t>Hoosier 20.5x6.0-13 R25B on 6 in. wide rim</t>
+  </si>
+  <si>
+    <t>Hoosier 20.5x7.0-13 R25B on 6 in. wide rim</t>
+  </si>
+  <si>
+    <t>Hoosier 20.0x7.5-13 R25B on 7 in. wide rim</t>
+  </si>
+  <si>
+    <t>Hoosier 20.0x7.5-13 R25B on 8 in. wide rim</t>
+  </si>
+  <si>
+    <t>Hoosier  6.0 / 18.0 - 10  LCO on 6 in. wide rim</t>
+  </si>
+  <si>
+    <t>Hoosier 20.5 x 7.0 13 R25B A2500 (Item 43163), 7 inch rim</t>
+  </si>
+  <si>
+    <t>Hoosier 20.5 x 7.0 13 R25B A2500 (Item 43163), 8 inch rim</t>
+  </si>
+  <si>
+    <t>Hoosier 18.0 x 7.5 10 R25B  (Item 43105), 7 inch rim</t>
+  </si>
+  <si>
+    <t>Hoosier 18.0 x 7.5 10 R25B  (Item 43105), 8 inch rim</t>
+  </si>
+  <si>
+    <t>Hoosier 43070 16x6-10 R25B, 6 inch rim</t>
+  </si>
+  <si>
+    <t>Hoosier 43070 16x6-10 LCO, 6 inch rim</t>
+  </si>
+  <si>
+    <t>Hoosier 43070 16x6-10 R25B, 7 inch rim</t>
+  </si>
+  <si>
+    <t>Hoosier 43075 16x7.5-10 LCO, 8 inch rim</t>
+  </si>
+  <si>
+    <t>Hoosier 43075 16x7.5-10 LCO, 7 inch rim</t>
+  </si>
+  <si>
+    <t>Hoosier 43070 16x6-10 LCO, 7 inch rim</t>
   </si>
 </sst>
 </file>
@@ -675,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7082005F-176C-489F-987E-F7C4B3533BA2}">
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,31 +715,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -744,10 +765,10 @@
         <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I2" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -773,10 +794,10 @@
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I3" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -802,7 +823,7 @@
         <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I4" t="s">
         <v>27</v>
@@ -831,7 +852,7 @@
         <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I5" t="s">
         <v>27</v>
@@ -860,7 +881,7 @@
         <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I6" t="s">
         <v>27</v>
@@ -889,7 +910,7 @@
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -915,7 +936,7 @@
         <v>6</v>
       </c>
       <c r="H8" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -941,7 +962,7 @@
         <v>6</v>
       </c>
       <c r="H9" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -967,7 +988,7 @@
         <v>6</v>
       </c>
       <c r="H10" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -993,7 +1014,7 @@
         <v>6</v>
       </c>
       <c r="H11" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1019,7 +1040,7 @@
         <v>6</v>
       </c>
       <c r="H12" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1045,7 +1066,7 @@
         <v>7</v>
       </c>
       <c r="H13" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1071,7 +1092,7 @@
         <v>8</v>
       </c>
       <c r="H14" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1097,7 +1118,7 @@
         <v>6</v>
       </c>
       <c r="H15" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I15" t="s">
         <v>27</v>
@@ -1126,7 +1147,7 @@
         <v>7</v>
       </c>
       <c r="H16" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I16" t="s">
         <v>27</v>
@@ -1155,7 +1176,7 @@
         <v>8</v>
       </c>
       <c r="H17" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I17" t="s">
         <v>27</v>
@@ -1184,7 +1205,7 @@
         <v>7</v>
       </c>
       <c r="H18" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I18" t="s">
         <v>27</v>
@@ -1213,7 +1234,7 @@
         <v>8</v>
       </c>
       <c r="H19" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I19" t="s">
         <v>27</v>
@@ -1242,10 +1263,10 @@
         <v>7</v>
       </c>
       <c r="H20" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="I20" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1271,10 +1292,10 @@
         <v>8</v>
       </c>
       <c r="H21" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="I21" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1285,7 +1306,7 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D22">
         <v>20</v>
@@ -1300,7 +1321,7 @@
         <v>7</v>
       </c>
       <c r="H22" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1311,7 +1332,7 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D23">
         <v>20</v>
@@ -1326,12 +1347,12 @@
         <v>8</v>
       </c>
       <c r="H23" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -1352,13 +1373,13 @@
         <v>7</v>
       </c>
       <c r="H24" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="B25">
         <v>4</v>
@@ -1379,13 +1400,13 @@
         <v>8</v>
       </c>
       <c r="H25" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -1406,15 +1427,15 @@
         <v>7</v>
       </c>
       <c r="H26" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="I26" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="B27">
         <v>4</v>
@@ -1435,15 +1456,15 @@
         <v>8</v>
       </c>
       <c r="H27" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="I27" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="B28">
         <v>4</v>
@@ -1461,10 +1482,10 @@
         <v>13</v>
       </c>
       <c r="G28">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H28" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I28" t="s">
         <v>13</v>
@@ -1472,7 +1493,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="B29">
         <v>4</v>
@@ -1490,10 +1511,10 @@
         <v>13</v>
       </c>
       <c r="G29">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H29" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I29" t="s">
         <v>13</v>
@@ -1501,7 +1522,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="B30">
         <v>4</v>
@@ -1519,10 +1540,10 @@
         <v>13</v>
       </c>
       <c r="G30">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H30" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I30" t="s">
         <v>13</v>
@@ -1530,7 +1551,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="B31">
         <v>4</v>
@@ -1548,10 +1569,10 @@
         <v>13</v>
       </c>
       <c r="G31">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H31" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I31" t="s">
         <v>13</v>
@@ -1559,7 +1580,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="B32">
         <v>4</v>
@@ -1580,7 +1601,7 @@
         <v>7</v>
       </c>
       <c r="H32" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I32" t="s">
         <v>13</v>
@@ -1588,7 +1609,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -1609,7 +1630,7 @@
         <v>8</v>
       </c>
       <c r="H33" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I33" t="s">
         <v>13</v>
@@ -1617,7 +1638,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B34">
         <v>5</v>
@@ -1638,15 +1659,15 @@
         <v>7</v>
       </c>
       <c r="H34" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I34" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B35">
         <v>5</v>
@@ -1667,15 +1688,15 @@
         <v>8</v>
       </c>
       <c r="H35" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I35" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B36">
         <v>5</v>
@@ -1696,12 +1717,12 @@
         <v>7</v>
       </c>
       <c r="H36" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B37">
         <v>5</v>
@@ -1722,12 +1743,12 @@
         <v>8</v>
       </c>
       <c r="H37" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B38">
         <v>5</v>
@@ -1748,7 +1769,7 @@
         <v>6</v>
       </c>
       <c r="H38" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I38" t="s">
         <v>13</v>
@@ -1756,7 +1777,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B39">
         <v>5</v>
@@ -1777,7 +1798,7 @@
         <v>7</v>
       </c>
       <c r="H39" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I39" t="s">
         <v>13</v>
@@ -1785,7 +1806,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B40">
         <v>5</v>
@@ -1806,7 +1827,7 @@
         <v>6</v>
       </c>
       <c r="H40" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I40" t="s">
         <v>13</v>
@@ -1814,7 +1835,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B41">
         <v>5</v>
@@ -1835,7 +1856,7 @@
         <v>7</v>
       </c>
       <c r="H41" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I41" t="s">
         <v>13</v>
@@ -1843,7 +1864,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B42">
         <v>5</v>
@@ -1864,7 +1885,7 @@
         <v>6</v>
       </c>
       <c r="H42" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I42" t="s">
         <v>14</v>
@@ -1872,7 +1893,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="B43">
         <v>5</v>
@@ -1890,10 +1911,10 @@
         <v>10</v>
       </c>
       <c r="G43">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H43" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I43" t="s">
         <v>14</v>
@@ -1901,36 +1922,36 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C44" t="s">
         <v>9</v>
       </c>
       <c r="D44">
-        <v>20.5</v>
+        <v>18</v>
       </c>
       <c r="E44">
         <v>6</v>
       </c>
       <c r="F44">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G44">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H44" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B45">
         <v>6</v>
@@ -1948,10 +1969,10 @@
         <v>13</v>
       </c>
       <c r="G45">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H45" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I45" t="s">
         <v>13</v>
@@ -1959,7 +1980,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B46">
         <v>6</v>
@@ -1971,16 +1992,16 @@
         <v>20.5</v>
       </c>
       <c r="E46">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46">
         <v>13</v>
       </c>
       <c r="G46">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H46" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I46" t="s">
         <v>13</v>
@@ -1988,7 +2009,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="B47">
         <v>6</v>
@@ -2009,7 +2030,7 @@
         <v>7</v>
       </c>
       <c r="H47" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I47" t="s">
         <v>13</v>
@@ -2017,33 +2038,36 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="B48">
         <v>6</v>
       </c>
       <c r="C48" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D48">
-        <v>20</v>
+        <v>20.5</v>
       </c>
       <c r="E48">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F48">
         <v>13</v>
       </c>
       <c r="G48">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H48" t="s">
-        <v>77</v>
+        <v>67</v>
+      </c>
+      <c r="I48" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B49">
         <v>6</v>
@@ -2061,44 +2085,41 @@
         <v>13</v>
       </c>
       <c r="G49">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H49" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B50">
         <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D50">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E50">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="F50">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G50">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H50" t="s">
-        <v>81</v>
-      </c>
-      <c r="I50" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="B51">
         <v>6</v>
@@ -2116,10 +2137,10 @@
         <v>10</v>
       </c>
       <c r="G51">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H51" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I51" t="s">
         <v>13</v>
@@ -2127,7 +2148,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="B52">
         <v>6</v>
@@ -2139,16 +2160,16 @@
         <v>18</v>
       </c>
       <c r="E52">
-        <v>6</v>
+        <v>7.5</v>
       </c>
       <c r="F52">
         <v>10</v>
       </c>
       <c r="G52">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H52" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I52" t="s">
         <v>13</v>
@@ -2156,7 +2177,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B53">
         <v>6</v>
@@ -2174,10 +2195,10 @@
         <v>10</v>
       </c>
       <c r="G53">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H53" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I53" t="s">
         <v>13</v>
@@ -2185,7 +2206,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B54">
         <v>6</v>
@@ -2203,18 +2224,18 @@
         <v>10</v>
       </c>
       <c r="G54">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H54" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I54" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B55">
         <v>6</v>
@@ -2232,10 +2253,10 @@
         <v>10</v>
       </c>
       <c r="G55">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H55" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I55" t="s">
         <v>14</v>
@@ -2243,19 +2264,19 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B56">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D56">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E56">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56">
         <v>10</v>
@@ -2264,15 +2285,15 @@
         <v>7</v>
       </c>
       <c r="H56" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I56" t="s">
-        <v>80</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B57">
         <v>7</v>
@@ -2290,18 +2311,18 @@
         <v>10</v>
       </c>
       <c r="G57">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H57" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I57" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B58">
         <v>7</v>
@@ -2310,27 +2331,27 @@
         <v>10</v>
       </c>
       <c r="D58">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E58">
-        <v>8.1999999999999993</v>
+        <v>7</v>
       </c>
       <c r="F58">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G58">
         <v>8</v>
       </c>
       <c r="H58" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I58" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B59">
         <v>7</v>
@@ -2348,18 +2369,18 @@
         <v>13</v>
       </c>
       <c r="G59">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H59" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I59" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B60">
         <v>7</v>
@@ -2371,24 +2392,24 @@
         <v>20</v>
       </c>
       <c r="E60">
-        <v>7.2</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="F60">
         <v>13</v>
       </c>
       <c r="G60">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H60" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I60" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B61">
         <v>7</v>
@@ -2406,18 +2427,18 @@
         <v>13</v>
       </c>
       <c r="G61">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H61" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I61" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B62">
         <v>7</v>
@@ -2429,24 +2450,24 @@
         <v>20</v>
       </c>
       <c r="E62">
-        <v>6.2</v>
+        <v>7.2</v>
       </c>
       <c r="F62">
         <v>13</v>
       </c>
       <c r="G62">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H62" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I62" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B63">
         <v>7</v>
@@ -2464,47 +2485,47 @@
         <v>13</v>
       </c>
       <c r="G63">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H63" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I63" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B64">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C64" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D64">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E64">
-        <v>7.5</v>
+        <v>6.2</v>
       </c>
       <c r="F64">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G64">
         <v>7</v>
       </c>
       <c r="H64" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I64" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="B65">
         <v>8</v>
@@ -2522,10 +2543,10 @@
         <v>10</v>
       </c>
       <c r="G65">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H65" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I65" t="s">
         <v>13</v>
@@ -2533,7 +2554,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B66">
         <v>8</v>
@@ -2545,16 +2566,16 @@
         <v>16</v>
       </c>
       <c r="E66">
-        <v>6</v>
+        <v>7.5</v>
       </c>
       <c r="F66">
         <v>10</v>
       </c>
       <c r="G66">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H66" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I66" t="s">
         <v>13</v>
@@ -2562,7 +2583,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="B67">
         <v>8</v>
@@ -2580,10 +2601,10 @@
         <v>10</v>
       </c>
       <c r="G67">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H67" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I67" t="s">
         <v>13</v>
@@ -2591,7 +2612,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="B68">
         <v>8</v>
@@ -2603,24 +2624,24 @@
         <v>16</v>
       </c>
       <c r="E68">
-        <v>7.5</v>
+        <v>6</v>
       </c>
       <c r="F68">
         <v>10</v>
       </c>
       <c r="G68">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H68" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I68" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="B69">
         <v>8</v>
@@ -2638,10 +2659,10 @@
         <v>10</v>
       </c>
       <c r="G69">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H69" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I69" t="s">
         <v>14</v>
@@ -2649,7 +2670,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="B70">
         <v>8</v>
@@ -2661,16 +2682,16 @@
         <v>16</v>
       </c>
       <c r="E70">
-        <v>6</v>
+        <v>7.5</v>
       </c>
       <c r="F70">
         <v>10</v>
       </c>
       <c r="G70">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H70" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I70" t="s">
         <v>14</v>
@@ -2678,7 +2699,7 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -2696,10 +2717,10 @@
         <v>10</v>
       </c>
       <c r="G71">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H71" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I71" t="s">
         <v>14</v>
@@ -2707,45 +2728,48 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="B72">
         <v>8</v>
       </c>
       <c r="C72" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D72">
-        <v>18.5</v>
+        <v>16</v>
       </c>
       <c r="E72">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F72">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G72">
         <v>7</v>
       </c>
       <c r="H72" t="s">
-        <v>77</v>
+        <v>67</v>
+      </c>
+      <c r="I72" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B73">
         <v>8</v>
       </c>
       <c r="C73" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D73">
-        <v>20</v>
+        <v>18.5</v>
       </c>
       <c r="E73">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F73">
         <v>13</v>
@@ -2754,12 +2778,12 @@
         <v>7</v>
       </c>
       <c r="H73" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B74">
         <v>8</v>
@@ -2777,10 +2801,36 @@
         <v>13</v>
       </c>
       <c r="G74">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H74" t="s">
-        <v>81</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>60</v>
+      </c>
+      <c r="B75">
+        <v>8</v>
+      </c>
+      <c r="C75" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75">
+        <v>20</v>
+      </c>
+      <c r="E75">
+        <v>7</v>
+      </c>
+      <c r="F75">
+        <v>13</v>
+      </c>
+      <c r="G75">
+        <v>8</v>
+      </c>
+      <c r="H75" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>